<commit_message>
removed auth from create user to test
</commit_message>
<xml_diff>
--- a/docs/User stories.xlsx
+++ b/docs/User stories.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jan\Documents\GC06\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jan\GC06Databases\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -146,9 +146,6 @@
     <t>change_password(username, password)</t>
   </si>
   <si>
-    <t>create_user(username, user_id, first_name, last_name, email, is_buyer, is_seller, password)</t>
-  </si>
-  <si>
     <t>get_auctions_feed()</t>
   </si>
   <si>
@@ -156,6 +153,9 @@
   </si>
   <si>
     <t>Stored Procedures</t>
+  </si>
+  <si>
+    <t>create_user(username, first_name, last_name, email, password)</t>
   </si>
 </sst>
 </file>
@@ -581,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -599,7 +599,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -615,7 +615,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -633,7 +633,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -668,7 +668,7 @@
         <v>19</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>